<commit_message>
move func in yolov5.py to utils.py
</commit_message>
<xml_diff>
--- a/logs_yolo/results.xlsx
+++ b/logs_yolo/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA48"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4265,6 +4265,91 @@
         <v>3072</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-02-14_23-21-55</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>yolov5</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>8</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1024</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2400</v>
+      </c>
+      <c r="F49" t="n">
+        <v>600</v>
+      </c>
+      <c r="G49" t="n">
+        <v>10</v>
+      </c>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>0.018909</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.026391</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.0054985</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.53124</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.77271</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.6584</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.33023</v>
+      </c>
+      <c r="P49" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>1</v>
+      </c>
+      <c r="R49" t="n">
+        <v>522.0679485999999</v>
+      </c>
+      <c r="S49" t="n">
+        <v>30</v>
+      </c>
+      <c r="T49" t="n">
+        <v>50</v>
+      </c>
+      <c r="U49" t="n">
+        <v>3072</v>
+      </c>
+      <c r="V49" t="n">
+        <v>1e-07</v>
+      </c>
+      <c r="W49" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="X49" t="n">
+        <v>131.4</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>0.00016</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>1.019271325721766e-07</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>3072</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>